<commit_message>
feat: added weekend only feature
</commit_message>
<xml_diff>
--- a/python/fare-filing/fare_input_backup.xlsx
+++ b/python/fare-filing/fare_input_backup.xlsx
@@ -518,7 +518,6 @@
       <c r="D2" t="n">
         <v>3400</v>
       </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -539,7 +538,6 @@
       <c r="D3" t="n">
         <v>4100</v>
       </c>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -560,7 +558,6 @@
       <c r="D4" t="n">
         <v>4200</v>
       </c>
-      <c r="E4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -573,7 +570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,6 +604,16 @@
           <t>direct</t>
         </is>
       </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 7</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -616,7 +623,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>J</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -625,9 +632,11 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2700</v>
+        <v>9765</v>
       </c>
       <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -637,7 +646,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -646,19 +655,21 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2800</v>
+        <v>7800</v>
       </c>
       <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SGN</t>
+          <t>TPE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -667,9 +678,11 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3500</v>
+        <v>5700</v>
       </c>
       <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -736,7 +749,6 @@
       <c r="D2" t="n">
         <v>3600</v>
       </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -757,7 +769,6 @@
       <c r="D3" t="n">
         <v>4300</v>
       </c>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -778,7 +789,6 @@
       <c r="D4" t="n">
         <v>4400</v>
       </c>
-      <c r="E4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -791,7 +801,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -825,6 +835,16 @@
           <t>direct</t>
         </is>
       </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 7</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -834,7 +854,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>J</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -843,9 +863,11 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2900</v>
+        <v>10120</v>
       </c>
       <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -855,7 +877,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -864,19 +886,21 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3000</v>
+        <v>8030</v>
       </c>
       <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SGN</t>
+          <t>TPE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -885,51 +909,11 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3700</v>
+        <v>5900</v>
       </c>
       <c r="E4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>SGN</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>3800</v>
-      </c>
-      <c r="E5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>BKK</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>4500</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -942,7 +926,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -976,6 +960,16 @@
           <t>direct</t>
         </is>
       </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 7</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -985,7 +979,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>J</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -994,9 +988,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2300</v>
+        <v>9275</v>
       </c>
       <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Remarks:
+'O' for One Season</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1006,7 +1007,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1015,9 +1016,11 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2400</v>
+        <v>7430</v>
       </c>
       <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1027,7 +1030,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1036,72 +1039,11 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3100</v>
+        <v>5400</v>
       </c>
       <c r="E4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>SGN</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>3200</v>
-      </c>
-      <c r="E5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>BKK</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>3900</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>BKK</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>4000</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1114,7 +1056,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1148,6 +1090,16 @@
           <t>direct</t>
         </is>
       </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 7</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1157,7 +1109,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>J</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1166,9 +1118,11 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2500</v>
+        <v>9655</v>
       </c>
       <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1178,7 +1132,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1187,19 +1141,21 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2600</v>
+        <v>7720</v>
       </c>
       <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SGN</t>
+          <t>TPE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1208,9 +1164,11 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3300</v>
+        <v>5630</v>
       </c>
       <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>